<commit_message>
nearly completes BLAST on new merged taxa table
</commit_message>
<xml_diff>
--- a/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-merged.xlsx
+++ b/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-merged.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57484E7-7C79-49E8-A6B3-B8A35D68487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{A57484E7-7C79-49E8-A6B3-B8A35D68487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4DD59C9-05D6-477A-936A-F6E290990D3D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="343">
   <si>
     <t>rownames</t>
   </si>
@@ -977,14 +977,86 @@
     <t>BLAST Notes</t>
   </si>
   <si>
-    <t>100% Myoxocephalus thompsonii, M. aeneas, M. scorpus, M. quadricornis</t>
+    <t>100% Myoxocephalus thompsonii, M. aeneaus, M. scorpius, M. quadricornis</t>
+  </si>
+  <si>
+    <t>100% Gymnocanthus intermedius AND Gymnocanthus pistilliger</t>
+  </si>
+  <si>
+    <t>100% Liparisochotensis AND Liparis gibbus</t>
+  </si>
+  <si>
+    <t>&gt;99% Myoxocephalus jaok, Myoxocephalus stelleri, Myoxocephalus polyacanthocephalus</t>
+  </si>
+  <si>
+    <t>&gt;99% Eleginus gracilis AND Micrpgadus proximus</t>
+  </si>
+  <si>
+    <t>100% Myoxocephalus jaok, Myoxocephalus stelleri, Myoxocephalus polyacanthocephalus</t>
+  </si>
+  <si>
+    <t>100% Hemilepidotus jordani, Hemilepidotus papilio</t>
+  </si>
+  <si>
+    <t>&gt;99% Clupea pallasii AND Clupea harengus</t>
+  </si>
+  <si>
+    <t>100% Liparis ochotensis AND Liparis gibbus</t>
+  </si>
+  <si>
+    <t>100% Lepidopsetta bilineata AND Lepidopsetta polyxystra</t>
+  </si>
+  <si>
+    <t>NO MATCH TO MYOXOCEPHALUS --&gt; PUNGITUS SPP. !!!!</t>
+  </si>
+  <si>
+    <t>Elegiunus gracilis</t>
+  </si>
+  <si>
+    <t>&gt; 99% Lumpenus fabricii AND Leptoclinus maculatus</t>
+  </si>
+  <si>
+    <t>NO SIGNIFICANT MATCHES FOUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% Sarritor leptorhynchus, Sarritor frenatus, Leptagonus decagonus, Podothecus veternus </t>
+  </si>
+  <si>
+    <t>&gt;99% to many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;99% Glyptocephalus zachirus, Glyptocephalus stelleri, Myzopsetta proboscidea, </t>
+  </si>
+  <si>
+    <t>&gt; 99% Myoxocephalus thompsonii, M. aeneaus, M. scorpius, M. quadricornis</t>
+  </si>
+  <si>
+    <t>all 100% matches to coregonus spp except 1 to Stenodus leucichthys</t>
+  </si>
+  <si>
+    <t>&gt;995 match to many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% Liparis ochotensis, Liparis gibbus, Liparis bathyarcticus </t>
+  </si>
+  <si>
+    <t>100% Brachyopsis segaliensis, occella dodaecaedron, Chesonia verrucosa</t>
+  </si>
+  <si>
+    <t>98% Gasterosteus aculeatus AND Gasterosteus nipponicus</t>
+  </si>
+  <si>
+    <t>&gt;99% Oncorhynchus gorbuscha</t>
+  </si>
+  <si>
+    <t>&gt;99% Oncorhynchus keta AND Oncorhynchus kisutch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1000,13 +1072,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1018,16 +1132,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1336,20 +1461,20 @@
       <selection activeCell="F187" sqref="F187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.06640625" customWidth="1"/>
-    <col min="3" max="3" width="14.86328125" customWidth="1"/>
-    <col min="4" max="4" width="14.9296875" customWidth="1"/>
-    <col min="5" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
-    <col min="7" max="7" width="17.1328125" customWidth="1"/>
-    <col min="8" max="8" width="24.19921875" customWidth="1"/>
-    <col min="9" max="9" width="16.796875" customWidth="1"/>
-    <col min="10" max="10" width="20.796875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1407,7 +1532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1439,7 +1564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1465,7 +1590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1497,7 +1622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1523,7 +1648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1549,7 +1674,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1581,7 +1706,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1592,7 +1717,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -1624,7 +1749,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1650,7 +1775,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1676,7 +1801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1702,7 +1827,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1722,7 +1847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1754,7 +1879,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1780,7 +1905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1812,7 +1937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1838,7 +1963,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -1864,7 +1989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1890,7 +2015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1916,7 +2041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1942,7 +2067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1968,7 +2093,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1991,7 +2116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -2023,7 +2148,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -2043,7 +2168,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -2066,7 +2191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -2092,7 +2217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2118,7 +2243,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -2150,7 +2275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -2176,7 +2301,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2199,7 +2324,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -2231,7 +2356,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2257,7 +2382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -2283,7 +2408,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -2309,7 +2434,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>93</v>
       </c>
@@ -2341,7 +2466,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -2361,7 +2486,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -2384,7 +2509,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -2410,7 +2535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -2430,7 +2555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2462,7 +2587,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -2488,7 +2613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -2520,7 +2645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -2546,7 +2671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2566,7 +2691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -2586,7 +2711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>109</v>
       </c>
@@ -2618,7 +2743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>110</v>
       </c>
@@ -2644,7 +2769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -2670,7 +2795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -2702,7 +2827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>113</v>
       </c>
@@ -2734,7 +2859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>114</v>
       </c>
@@ -2760,7 +2885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -2786,7 +2911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>116</v>
       </c>
@@ -2812,7 +2937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>117</v>
       </c>
@@ -2832,7 +2957,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>118</v>
       </c>
@@ -2855,7 +2980,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>120</v>
       </c>
@@ -2884,7 +3009,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>122</v>
       </c>
@@ -2904,7 +3029,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -2930,7 +3055,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>126</v>
       </c>
@@ -2956,7 +3081,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>129</v>
       </c>
@@ -2982,7 +3107,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>130</v>
       </c>
@@ -3002,7 +3127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>131</v>
       </c>
@@ -3022,7 +3147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -3048,7 +3173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -3080,7 +3205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -3100,7 +3225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -3120,7 +3245,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -3140,7 +3265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>137</v>
       </c>
@@ -3163,7 +3288,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -3192,7 +3317,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>143</v>
       </c>
@@ -3212,7 +3337,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -3238,7 +3363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -3264,7 +3389,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -3296,7 +3421,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -3307,7 +3432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>151</v>
       </c>
@@ -3339,7 +3464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -3359,7 +3484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -3391,7 +3516,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -3411,7 +3536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>155</v>
       </c>
@@ -3437,7 +3562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>156</v>
       </c>
@@ -3463,7 +3588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>157</v>
       </c>
@@ -3495,7 +3620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -3521,7 +3646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>159</v>
       </c>
@@ -3532,7 +3657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>160</v>
       </c>
@@ -3558,7 +3683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>161</v>
       </c>
@@ -3584,7 +3709,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>164</v>
       </c>
@@ -3610,7 +3735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>165</v>
       </c>
@@ -3630,7 +3755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>166</v>
       </c>
@@ -3662,7 +3787,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -3679,7 +3804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>168</v>
       </c>
@@ -3699,7 +3824,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -3731,7 +3856,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>170</v>
       </c>
@@ -3751,7 +3876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>171</v>
       </c>
@@ -3777,7 +3902,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>172</v>
       </c>
@@ -3788,7 +3913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>173</v>
       </c>
@@ -3808,7 +3933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>174</v>
       </c>
@@ -3831,7 +3956,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>175</v>
       </c>
@@ -3854,7 +3979,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>177</v>
       </c>
@@ -3874,7 +3999,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>178</v>
       </c>
@@ -3894,7 +4019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>179</v>
       </c>
@@ -3920,7 +4045,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>180</v>
       </c>
@@ -3946,7 +4071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>181</v>
       </c>
@@ -3975,7 +4100,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>183</v>
       </c>
@@ -4007,7 +4132,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>184</v>
       </c>
@@ -4027,7 +4152,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>185</v>
       </c>
@@ -4059,7 +4184,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>186</v>
       </c>
@@ -4085,7 +4210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>187</v>
       </c>
@@ -4105,7 +4230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>188</v>
       </c>
@@ -4125,7 +4250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>189</v>
       </c>
@@ -4157,7 +4282,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>192</v>
       </c>
@@ -4183,7 +4308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>193</v>
       </c>
@@ -4212,7 +4337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>194</v>
       </c>
@@ -4241,7 +4366,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>196</v>
       </c>
@@ -4267,7 +4392,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>200</v>
       </c>
@@ -4299,7 +4424,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>204</v>
       </c>
@@ -4325,7 +4450,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>205</v>
       </c>
@@ -4345,7 +4470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>206</v>
       </c>
@@ -4377,7 +4502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>207</v>
       </c>
@@ -4409,7 +4534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>208</v>
       </c>
@@ -4441,7 +4566,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>209</v>
       </c>
@@ -4467,7 +4592,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>214</v>
       </c>
@@ -4478,7 +4603,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>216</v>
       </c>
@@ -4504,7 +4629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>217</v>
       </c>
@@ -4530,7 +4655,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>218</v>
       </c>
@@ -4550,7 +4675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>219</v>
       </c>
@@ -4582,7 +4707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>220</v>
       </c>
@@ -4611,7 +4736,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -4634,7 +4759,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>223</v>
       </c>
@@ -4645,7 +4770,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>225</v>
       </c>
@@ -4668,7 +4793,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>226</v>
       </c>
@@ -4700,7 +4825,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>227</v>
       </c>
@@ -4732,7 +4857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>228</v>
       </c>
@@ -4758,7 +4883,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>230</v>
       </c>
@@ -4775,7 +4900,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>231</v>
       </c>
@@ -4795,7 +4920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>232</v>
       </c>
@@ -4827,7 +4952,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>236</v>
       </c>
@@ -4859,7 +4984,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>237</v>
       </c>
@@ -4891,7 +5016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>238</v>
       </c>
@@ -4911,7 +5036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>239</v>
       </c>
@@ -4943,7 +5068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>240</v>
       </c>
@@ -4957,7 +5082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>241</v>
       </c>
@@ -4968,7 +5093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>242</v>
       </c>
@@ -4994,7 +5119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>243</v>
       </c>
@@ -5026,7 +5151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>244</v>
       </c>
@@ -5058,7 +5183,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>245</v>
       </c>
@@ -5090,7 +5215,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>246</v>
       </c>
@@ -5104,7 +5229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>247</v>
       </c>
@@ -5121,7 +5246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>248</v>
       </c>
@@ -5153,7 +5278,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>251</v>
       </c>
@@ -5185,7 +5310,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>254</v>
       </c>
@@ -5196,7 +5321,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>255</v>
       </c>
@@ -5228,7 +5353,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>256</v>
       </c>
@@ -5254,7 +5379,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>257</v>
       </c>
@@ -5286,7 +5411,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>258</v>
       </c>
@@ -5318,7 +5443,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>261</v>
       </c>
@@ -5344,7 +5469,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>262</v>
       </c>
@@ -5355,7 +5480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>263</v>
       </c>
@@ -5381,7 +5506,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>264</v>
       </c>
@@ -5413,7 +5538,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>265</v>
       </c>
@@ -5445,7 +5570,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>266</v>
       </c>
@@ -5456,7 +5581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>267</v>
       </c>
@@ -5488,7 +5613,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>268</v>
       </c>
@@ -5520,7 +5645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>269</v>
       </c>
@@ -5552,7 +5677,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>271</v>
       </c>
@@ -5563,7 +5688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>272</v>
       </c>
@@ -5595,7 +5720,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>274</v>
       </c>
@@ -5615,7 +5740,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>275</v>
       </c>
@@ -5641,7 +5766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>276</v>
       </c>
@@ -5673,7 +5798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>277</v>
       </c>
@@ -5693,7 +5818,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>278</v>
       </c>
@@ -5725,7 +5850,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>282</v>
       </c>
@@ -5754,7 +5879,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>287</v>
       </c>
@@ -5786,7 +5911,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>291</v>
       </c>
@@ -5818,7 +5943,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>294</v>
       </c>
@@ -5850,7 +5975,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>297</v>
       </c>
@@ -5882,7 +6007,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>298</v>
       </c>
@@ -5893,7 +6018,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>299</v>
       </c>
@@ -5913,7 +6038,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>300</v>
       </c>
@@ -5945,7 +6070,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>305</v>
       </c>
@@ -5977,7 +6102,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>308</v>
       </c>
@@ -5988,7 +6113,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>311</v>
       </c>
@@ -6014,7 +6139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>312</v>
       </c>
@@ -6040,7 +6165,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>315</v>
       </c>
@@ -6072,7 +6197,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>316</v>
       </c>
@@ -6101,23 +6226,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833455E8-1F45-4872-A5D0-55AA805A6B3E}">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.53125" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="59.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="59.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6152,7 +6277,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -6181,7 +6306,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -6200,8 +6325,11 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -6232,8 +6360,11 @@
       <c r="J4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -6264,34 +6395,40 @@
       <c r="J5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="K5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -6314,27 +6451,30 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -6356,8 +6496,11 @@
       <c r="G9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -6382,8 +6525,11 @@
       <c r="I10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K10" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -6405,8 +6551,11 @@
       <c r="J11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>88</v>
       </c>
@@ -6431,34 +6580,40 @@
       <c r="H12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="K12" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -6489,28 +6644,34 @@
       <c r="J14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="K14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -6532,327 +6693,369 @@
       <c r="I16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="K16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="K17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+      <c r="K18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="K19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="K23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="K24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="K25" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="K26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="K28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="K29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -6872,47 +7075,53 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="B32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="K32" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K33" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -6931,8 +7140,11 @@
       <c r="F34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>150</v>
       </c>
@@ -6942,74 +7154,86 @@
       <c r="C35" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="K35" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="K36" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="B37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+      <c r="K37" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B38" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="B38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K38" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>159</v>
       </c>
@@ -7019,28 +7243,34 @@
       <c r="C39" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="K39" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="B40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K40" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>167</v>
       </c>
@@ -7056,8 +7286,11 @@
       <c r="E41" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K41" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>168</v>
       </c>
@@ -7076,28 +7309,34 @@
       <c r="F42" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="K42" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="B43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K43" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>172</v>
       </c>
@@ -7107,8 +7346,11 @@
       <c r="C44" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K44" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>173</v>
       </c>
@@ -7127,8 +7369,11 @@
       <c r="F45" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K45" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>174</v>
       </c>
@@ -7150,31 +7395,37 @@
       <c r="G46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="K46" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K47" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>177</v>
       </c>
@@ -7193,109 +7444,121 @@
       <c r="F48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="K48" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="K49" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="B50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="K50" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="52" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="B52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K52" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>184</v>
       </c>
@@ -7314,8 +7577,11 @@
       <c r="F53" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K53" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>185</v>
       </c>
@@ -7346,100 +7612,115 @@
       <c r="J54" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="K54" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B55" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="B55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="K55" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B56" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="B56" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="K56" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B57" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="B57" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="K57" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H58" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K58" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -7467,80 +7748,89 @@
       <c r="J59" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="K59" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B60" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="B60" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H60" s="5" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="K60" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B61" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="B61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+    <row r="62" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="B62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K62" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>209</v>
       </c>
@@ -7565,39 +7855,48 @@
       <c r="J63" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+      <c r="K63" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J64" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+      <c r="K64" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B65" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="B65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K65" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>222</v>
       </c>
@@ -7619,68 +7918,77 @@
       <c r="G66" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="K66" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J67" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+      <c r="K67" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C68" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="B68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="K68" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B69" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="B69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J69" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>230</v>
       </c>
@@ -7697,7 +8005,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>231</v>
       </c>
@@ -7717,7 +8025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>236</v>
       </c>
@@ -7749,7 +8057,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>238</v>
       </c>
@@ -7769,7 +8077,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>240</v>
       </c>
@@ -7783,7 +8091,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>241</v>
       </c>
@@ -7794,7 +8102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>246</v>
       </c>
@@ -7808,7 +8116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>247</v>
       </c>
@@ -7825,7 +8133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>254</v>
       </c>
@@ -7836,7 +8144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>257</v>
       </c>
@@ -7868,7 +8176,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>261</v>
       </c>
@@ -7894,7 +8202,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>262</v>
       </c>
@@ -7905,7 +8213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>264</v>
       </c>
@@ -7937,7 +8245,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>265</v>
       </c>
@@ -7969,7 +8277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>266</v>
       </c>
@@ -7980,7 +8288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>267</v>
       </c>
@@ -8012,7 +8320,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>271</v>
       </c>
@@ -8023,7 +8331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>272</v>
       </c>
@@ -8055,7 +8363,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>274</v>
       </c>
@@ -8075,7 +8383,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>282</v>
       </c>
@@ -8104,7 +8412,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>297</v>
       </c>
@@ -8136,7 +8444,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>298</v>
       </c>
@@ -8147,7 +8455,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>299</v>
       </c>
@@ -8167,7 +8475,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>308</v>
       </c>
@@ -8178,7 +8486,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>312</v>
       </c>

</xml_diff>